<commit_message>
Exportar Factor Reajuste -Estable-
</commit_message>
<xml_diff>
--- a/SOP_IAA/Plantillas/Informe_Descriptivo_Item.xlsx
+++ b/SOP_IAA/Plantillas/Informe_Descriptivo_Item.xlsx
@@ -73,7 +73,7 @@
     <numFmt numFmtId="167" formatCode="_(&quot;₡&quot;* #,##0.000_);_(&quot;₡&quot;* \(#,##0.000\);_(&quot;₡&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="#,##0.000_);\(#,##0.000\)"/>
-    <numFmt numFmtId="170" formatCode="[$₡-140A]#,##0.000_);\([$₡-140A]#,##0.000\)"/>
+    <numFmt numFmtId="171" formatCode="[$₡-140A]#,##0.0000_);\([$₡-140A]#,##0.0000\)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -418,12 +418,30 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="7" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -478,26 +496,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="39" fontId="7" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -809,7 +809,7 @@
   <dimension ref="D3:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,90 +826,90 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="41"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="47"/>
     </row>
     <row r="4" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="44"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="50"/>
     </row>
     <row r="5" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D5" s="45"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="53"/>
     </row>
     <row r="6" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="50"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="56"/>
     </row>
     <row r="7" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="50"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="56"/>
     </row>
     <row r="8" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D8" s="51"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="59"/>
     </row>
     <row r="9" spans="4:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="38"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="44"/>
     </row>
     <row r="10" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
@@ -948,34 +948,34 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="55" t="s">
+      <c r="E13" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="56" t="s">
+      <c r="G13" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="56" t="s">
+      <c r="H13" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="56" t="s">
+      <c r="I13" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="57" t="s">
+      <c r="J13" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="59" t="s">
+      <c r="L13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="60" t="s">
+      <c r="M13" s="41" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       <c r="G18" s="16"/>
       <c r="H18" s="17"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="34">
+      <c r="J18" s="60">
         <v>0</v>
       </c>
       <c r="K18" s="6"/>
@@ -1049,7 +1049,7 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="31"/>
@@ -1057,7 +1057,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="17"/>
       <c r="I19" s="18"/>
-      <c r="J19" s="34">
+      <c r="J19" s="60">
         <v>0</v>
       </c>
       <c r="K19" s="6"/>

</xml_diff>